<commit_message>
changes flow, botons, front
</commit_message>
<xml_diff>
--- a/xlsx/excel_tipo.xlsx
+++ b/xlsx/excel_tipo.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\nclientes\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp_8.0\htdocs\nclienves-v2\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2112C2-B481-4DD1-AB35-3F5A8EB2A56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07A6CBF-B4D2-49CF-B376-843BD22F6065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B46FB847-E97B-4DE4-8B22-2602FA5DB8E1}"/>
+    <workbookView xWindow="-22425" yWindow="1980" windowWidth="19875" windowHeight="12660" xr2:uid="{B46FB847-E97B-4DE4-8B22-2602FA5DB8E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$AZ$1:$AZ$123</definedName>
-    <definedName name="comuna">Hoja1!$AZ$2:$AZ$110</definedName>
-    <definedName name="comunas">Hoja1!$AZ$2:$AZ$74</definedName>
-    <definedName name="comunasv2">Hoja1!$AZ$2:$AZ$81</definedName>
-    <definedName name="listado">Hoja1!$AZ$2:$AZ$110</definedName>
-    <definedName name="new">Hoja1!$AZ$2:$AZ$79</definedName>
-    <definedName name="nuevas">Hoja1!$AZ$2:$AZ$78</definedName>
-    <definedName name="QuintaRM">Hoja1!$AZ$2:$AZ$86</definedName>
-    <definedName name="receptor">Hoja1!$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$BA$1:$BA$123</definedName>
+    <definedName name="comuna">Hoja1!$BA$2:$BA$110</definedName>
+    <definedName name="comunas">Hoja1!$BA$2:$BA$74</definedName>
+    <definedName name="comunasv2">Hoja1!$BA$2:$BA$81</definedName>
+    <definedName name="listado">Hoja1!$BA$2:$BA$110</definedName>
+    <definedName name="new">Hoja1!$BA$2:$BA$79</definedName>
+    <definedName name="nuevas">Hoja1!$BA$2:$BA$78</definedName>
+    <definedName name="QuintaRM">Hoja1!$BA$2:$BA$86</definedName>
+    <definedName name="receptor">Hoja1!$F$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,18 +47,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
-  <si>
-    <t>NOMBRE CLIENTE FINAL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>DIRECCION ENTREGA</t>
   </si>
   <si>
     <t>TELEFONO</t>
-  </si>
-  <si>
-    <t>Email cliente (opcion)</t>
   </si>
   <si>
     <t>COMUNA ENTREGA</t>
@@ -484,6 +478,15 @@
   </si>
   <si>
     <t>SAN FRANCISCO DE MOSTAZAL</t>
+  </si>
+  <si>
+    <t>RUT (sin punto ni guion)</t>
+  </si>
+  <si>
+    <t>NOMBRE DESTINATARIO</t>
+  </si>
+  <si>
+    <t>EMAIL CLIENTE</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -624,7 +627,6 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +661,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1247776</xdr:colOff>
+      <xdr:colOff>1400176</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>128524</xdr:rowOff>
     </xdr:to>
@@ -1000,120 +1002,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1933B38B-02BE-41ED-BD22-8D0AF84AF757}">
-  <dimension ref="A1:BA123"/>
+  <dimension ref="A1:BB123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="51" width="11.42578125" style="1"/>
-    <col min="52" max="52" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
+    <col min="10" max="52" width="11.42578125" style="1"/>
+    <col min="53" max="53" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="10"/>
+    <row r="1" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
-      <c r="AZ1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="C2" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="BA1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="AZ2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="D3" s="3"/>
+      <c r="I2" s="10"/>
+      <c r="BA2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="AZ3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9"/>
+      <c r="I3" s="3"/>
+      <c r="BA3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="3"/>
-      <c r="AZ4" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="AZ5" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I4" s="3"/>
+      <c r="BA4" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BA5" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AZ6" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA6" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1122,11 +1128,12 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="AZ7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="BA7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1135,11 +1142,12 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="AZ8" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="BA8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1148,11 +1156,12 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="AZ9" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
+      <c r="BA9" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1161,11 +1170,12 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="AZ10" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+      <c r="BA10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1174,11 +1184,12 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="AZ11" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+      <c r="BA11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1187,11 +1198,12 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="AZ12" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="BA12" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1200,11 +1212,12 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="AZ13" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+      <c r="BA13" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1213,11 +1226,12 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="AZ14" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="BA14" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1226,11 +1240,12 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="AZ15" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+      <c r="BA15" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1239,11 +1254,12 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="AZ16" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+      <c r="BA16" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1252,11 +1268,12 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="AZ17" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I17" s="2"/>
+      <c r="BA17" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1265,11 +1282,12 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="AZ18" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I18" s="2"/>
+      <c r="BA18" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1278,11 +1296,12 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="AZ19" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I19" s="2"/>
+      <c r="BA19" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1291,11 +1310,12 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="AZ20" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I20" s="2"/>
+      <c r="BA20" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1304,11 +1324,12 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="AZ21" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I21" s="2"/>
+      <c r="BA21" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1317,11 +1338,12 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="AZ22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I22" s="2"/>
+      <c r="BA22" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1330,11 +1352,12 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="AZ23" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I23" s="2"/>
+      <c r="BA23" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1343,11 +1366,12 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="AZ24" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I24" s="2"/>
+      <c r="BA24" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1356,11 +1380,12 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="AZ25" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I25" s="2"/>
+      <c r="BA25" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1369,11 +1394,12 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="AZ26" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I26" s="2"/>
+      <c r="BA26" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1382,11 +1408,12 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="AZ27" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I27" s="2"/>
+      <c r="BA27" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1395,11 +1422,12 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="AZ28" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I28" s="2"/>
+      <c r="BA28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1408,11 +1436,12 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="AZ29" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I29" s="2"/>
+      <c r="BA29" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1421,11 +1450,12 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="AZ30" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I30" s="2"/>
+      <c r="BA30" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1434,11 +1464,12 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="AZ31" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I31" s="2"/>
+      <c r="BA31" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1447,11 +1478,12 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="AZ32" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:52" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I32" s="2"/>
+      <c r="BA32" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1460,11 +1492,12 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="AZ33" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I33" s="2"/>
+      <c r="BA33" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1473,11 +1506,12 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="AZ34" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I34" s="2"/>
+      <c r="BA34" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1486,11 +1520,12 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="AZ35" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I35" s="2"/>
+      <c r="BA35" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1499,11 +1534,12 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="AZ36" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I36" s="2"/>
+      <c r="BA36" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1512,11 +1548,12 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="AZ37" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I37" s="2"/>
+      <c r="BA37" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1525,11 +1562,12 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="AZ38" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I38" s="2"/>
+      <c r="BA38" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1538,11 +1576,12 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="AZ39" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I39" s="2"/>
+      <c r="BA39" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1551,11 +1590,12 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="AZ40" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I40" s="2"/>
+      <c r="BA40" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1564,11 +1604,12 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="AZ41" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I41" s="2"/>
+      <c r="BA41" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1577,11 +1618,12 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-      <c r="AZ42" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I42" s="2"/>
+      <c r="BA42" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1590,11 +1632,12 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
-      <c r="AZ43" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I43" s="2"/>
+      <c r="BA43" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1603,11 +1646,12 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-      <c r="AZ44" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I44" s="2"/>
+      <c r="BA44" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1616,11 +1660,12 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="AZ45" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I45" s="2"/>
+      <c r="BA45" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1629,11 +1674,12 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-      <c r="AZ46" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I46" s="2"/>
+      <c r="BA46" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1642,11 +1688,12 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-      <c r="AZ47" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I47" s="2"/>
+      <c r="BA47" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1655,11 +1702,12 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
-      <c r="AZ48" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I48" s="2"/>
+      <c r="BA48" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1668,11 +1716,12 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
-      <c r="AZ49" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I49" s="2"/>
+      <c r="BA49" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1681,11 +1730,12 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
-      <c r="AZ50" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I50" s="2"/>
+      <c r="BA50" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1694,11 +1744,12 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
-      <c r="AZ51" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I51" s="2"/>
+      <c r="BA51" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1707,11 +1758,12 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
-      <c r="AZ52" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I52" s="2"/>
+      <c r="BA52" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1720,11 +1772,12 @@
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
-      <c r="AZ53" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I53" s="2"/>
+      <c r="BA53" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1733,11 +1786,12 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
-      <c r="AZ54" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I54" s="2"/>
+      <c r="BA54" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1746,11 +1800,12 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="AZ55" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I55" s="2"/>
+      <c r="BA55" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1759,11 +1814,12 @@
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
-      <c r="AZ56" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I56" s="2"/>
+      <c r="BA56" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1772,11 +1828,12 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
-      <c r="AZ57" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I57" s="2"/>
+      <c r="BA57" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1785,11 +1842,12 @@
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="AZ58" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I58" s="2"/>
+      <c r="BA58" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1798,11 +1856,12 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="AZ59" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I59" s="2"/>
+      <c r="BA59" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1811,11 +1870,12 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="AZ60" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I60" s="2"/>
+      <c r="BA60" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1824,11 +1884,12 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
-      <c r="AZ61" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I61" s="2"/>
+      <c r="BA61" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1837,11 +1898,12 @@
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
-      <c r="AZ62" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I62" s="2"/>
+      <c r="BA62" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1850,11 +1912,12 @@
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
-      <c r="AZ63" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I63" s="2"/>
+      <c r="BA63" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1863,11 +1926,12 @@
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
-      <c r="AZ64" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I64" s="2"/>
+      <c r="BA64" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1876,11 +1940,12 @@
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
-      <c r="AZ65" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I65" s="2"/>
+      <c r="BA65" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1889,11 +1954,12 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
-      <c r="AZ66" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="67" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I66" s="2"/>
+      <c r="BA66" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1902,11 +1968,12 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
-      <c r="AZ67" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I67" s="2"/>
+      <c r="BA67" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1915,11 +1982,12 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
-      <c r="AZ68" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I68" s="2"/>
+      <c r="BA68" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1928,11 +1996,12 @@
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
-      <c r="AZ69" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="70" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I69" s="2"/>
+      <c r="BA69" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1941,11 +2010,12 @@
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
-      <c r="AZ70" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I70" s="2"/>
+      <c r="BA70" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1954,11 +2024,12 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
-      <c r="AZ71" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="72" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I71" s="2"/>
+      <c r="BA71" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -1967,11 +2038,12 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
-      <c r="AZ72" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="73" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I72" s="2"/>
+      <c r="BA72" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1980,11 +2052,12 @@
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="AZ73" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I73" s="2"/>
+      <c r="BA73" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1993,11 +2066,12 @@
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
-      <c r="AZ74" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="75" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I74" s="2"/>
+      <c r="BA74" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2006,11 +2080,12 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
-      <c r="AZ75" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I75" s="2"/>
+      <c r="BA75" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2019,11 +2094,12 @@
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
-      <c r="AZ76" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="77" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I76" s="2"/>
+      <c r="BA76" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2032,11 +2108,12 @@
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
-      <c r="AZ77" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="78" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I77" s="2"/>
+      <c r="BA77" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="78" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2045,11 +2122,12 @@
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
-      <c r="AZ78" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I78" s="2"/>
+      <c r="BA78" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2058,11 +2136,12 @@
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
-      <c r="AZ79" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="80" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I79" s="2"/>
+      <c r="BA79" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2071,11 +2150,12 @@
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
-      <c r="AZ80" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="81" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I80" s="2"/>
+      <c r="BA80" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2084,11 +2164,12 @@
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
-      <c r="AZ81" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="82" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I81" s="2"/>
+      <c r="BA81" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="82" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2097,11 +2178,12 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
-      <c r="AZ82" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="83" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I82" s="2"/>
+      <c r="BA82" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2110,11 +2192,12 @@
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
-      <c r="AZ83" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="84" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I83" s="2"/>
+      <c r="BA83" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2123,11 +2206,12 @@
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
-      <c r="AZ84" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="85" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I84" s="2"/>
+      <c r="BA84" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2136,11 +2220,12 @@
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
-      <c r="AZ85" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="86" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I85" s="2"/>
+      <c r="BA85" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2149,11 +2234,12 @@
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
-      <c r="AZ86" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="87" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I86" s="2"/>
+      <c r="BA86" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="87" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2162,11 +2248,12 @@
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
-      <c r="AZ87" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="88" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I87" s="2"/>
+      <c r="BA87" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2175,11 +2262,12 @@
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
-      <c r="AZ88" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="89" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I88" s="2"/>
+      <c r="BA88" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2188,11 +2276,12 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
-      <c r="AZ89" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="90" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I89" s="2"/>
+      <c r="BA89" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2201,11 +2290,12 @@
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
-      <c r="AZ90" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="91" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I90" s="2"/>
+      <c r="BA90" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2214,11 +2304,12 @@
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
-      <c r="AZ91" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="92" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I91" s="2"/>
+      <c r="BA91" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="92" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2227,11 +2318,12 @@
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
-      <c r="AZ92" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="93" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I92" s="2"/>
+      <c r="BA92" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2240,11 +2332,12 @@
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
-      <c r="AZ93" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="94" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I93" s="2"/>
+      <c r="BA93" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2253,11 +2346,12 @@
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
-      <c r="AZ94" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="95" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I94" s="2"/>
+      <c r="BA94" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2266,11 +2360,12 @@
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
-      <c r="AZ95" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="96" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I95" s="2"/>
+      <c r="BA95" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2279,11 +2374,12 @@
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
-      <c r="AZ96" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="97" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I96" s="2"/>
+      <c r="BA96" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2292,11 +2388,12 @@
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
-      <c r="AZ97" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="98" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I97" s="2"/>
+      <c r="BA97" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="98" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2305,11 +2402,12 @@
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
-      <c r="AZ98" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="99" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I98" s="2"/>
+      <c r="BA98" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2318,11 +2416,12 @@
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
-      <c r="AZ99" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="100" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="I99" s="2"/>
+      <c r="BA99" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2331,141 +2430,142 @@
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
-      <c r="AZ100" s="1" t="s">
+      <c r="I100" s="2"/>
+      <c r="BA100" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA101" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA102" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="103" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA103" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA104" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA105" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="106" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA106" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="107" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA107" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ101" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ102" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="103" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ103" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="104" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ104" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ105" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="106" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ106" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="107" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ107" s="1" t="s">
+    <row r="108" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA108" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA109" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="110" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA110" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="111" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA111" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="112" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BA112" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA113" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="114" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA114" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="108" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ108" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="109" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ109" s="4" t="s">
+    <row r="115" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA115" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="116" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA116" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="117" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA117" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA118" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="119" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA119" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA120" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA121" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA122" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ110" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="111" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ111" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="112" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AZ112" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="113" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ113" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="114" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ114" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="115" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ115" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="116" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ116" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="117" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ117" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="118" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ118" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="119" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ119" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="120" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ120" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="121" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ121" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="122" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ122" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="123" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ123" s="11" t="s">
-        <v>74</v>
+    <row r="123" spans="53:53" x14ac:dyDescent="0.25">
+      <c r="BA123" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="AZ1:AZ123" xr:uid="{1933B38B-02BE-41ED-BD22-8D0AF84AF757}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AZ2:AZ123">
-      <sortCondition ref="AZ1:AZ123"/>
+  <autoFilter ref="BA1:BA123" xr:uid="{1933B38B-02BE-41ED-BD22-8D0AF84AF757}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="BA2:BA123">
+      <sortCondition ref="BA1:BA123"/>
     </sortState>
   </autoFilter>
   <mergeCells count="2">
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="D1:I2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E1048576" xr:uid="{76E85EC8-ECE8-48DD-B002-0A94E973ED23}">
-      <formula1>$AZ$2:$AZ$123</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F1048576" xr:uid="{76E85EC8-ECE8-48DD-B002-0A94E973ED23}">
+      <formula1>$BA$2:$BA$123</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1048576" xr:uid="{C9CC870B-093F-4921-90B4-76C81A729A8A}">
-      <formula1>$BA$2:$BA$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I1048576" xr:uid="{C9CC870B-093F-4921-90B4-76C81A729A8A}">
+      <formula1>$BB$2:$BB$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>